<commit_message>
changes to excel sheet for motor calcs
</commit_message>
<xml_diff>
--- a/Motor_calculations/Car calculations.xlsx
+++ b/Motor_calculations/Car calculations.xlsx
@@ -8,13 +8,68 @@
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet r:id="rId2" sheetId="2" name="Sheet2"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+  <si>
+    <t>Old motor options</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Photo</t>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>Battery</t>
+  </si>
+  <si>
+    <t>RPM</t>
+  </si>
+  <si>
+    <t>Torque (Nm)</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com.au/itm/316188680273?_trkparms=amclksrc=ITM%26aid=1110006%26algo=HOMESPLICE.SIM%26ao=1%26asc=284134,284158%26meid=1506fbf1089544e9821a2e167fe68cc4%26pid=101875%26rk=1%26rkt=4%26sd=306069865771%26itm=316188680273%26pmt=1%26noa=0%26pg=2332490%26algv=SimVIDwebV3WithCPCExpansionEmbeddingSearchQuerySemanticBroadMatchSingularityRecallReplaceKnnV4WithVectorDbNsOptHotPlRecallCIICentroidCoviewCPCAuto%26brand=Unbranded&amp;_trksid=p2332490.c101875.m1851&amp;itmprp=cksum%3A3161886802731506fbf1089544e9821a2e167fe68cc4|enc%3AAQAKAAABgG96wQ16jds4VFcrhy1F3d4mbwZUJI9Fs%252BgdXYAHIzlX2e3YaNh7x%252BEnKA3G%252BCqSl1Xn4McfcWFK1GytmS2qxJ87mtE8Gm3iR1Ja4WBwh0hNHJrJx3Ki5mp04ow4CO7lP%252BooCybZDDU%252BbbSwmg7CbTin%252BBzBzbCYVnbjvyQAHu6--HI4MB7SvJl5IJqlyvomgoLMlgT6qAJzX0SANJhty2cscUA3K%252FZdWzP42Dt%252FaT%252B8ZmIapzFrkwXSKca%252FlXLttQzzgZ8faZIvwSHUdc9AlegYmiwq3XqFb%252FV4%252F3pd4gFhpDsq5XmH3NoZQcMo04dP2CKdlAhtkoJ9ALMrkEeBrHTMiiN1xOV4EjLB2h1eoqvAQZ5VTxiwrcsqnDz7FJLwpyPV2ql6f6A3t1cWjw3Im%252F7FvxgFUVLz2D8z0NvgmyDKz%252BhLajNVDoKvoOERy65QTyd5aKP1%252Bu4cgH7GO%252FpSJZFmPn9Y3HpVKmXXPAkNOkc1q%252Bqbqp0852bxS%252FeNAT3wIA%253D%253D|ampid%3APL_CLK|clp%3A2332490&amp;itmmeta=01JS39S56M81NGMKCES2YX4CZ5</t>
+  </si>
+  <si>
+    <t>#VALUE!</t>
+  </si>
+  <si>
+    <t>2000W</t>
+  </si>
+  <si>
+    <t>12V</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com.au/itm/326442694096?_skw=blender+1000W+portable&amp;itmmeta=01JS3AZHME26F5MVNB03R9C01A&amp;hash=item4c018035d0:g:EZwAAOSwOaVnriH5&amp;itmprp=enc%3AAQAKAAAA0FkggFvd1GGDu0w3yXCmi1fxLO2niJwQP%2F5sA8z3Uwa41GimoIY1BKtBB9nGFL7R+bf4dkU34guuFw6hXCCQUbFlGW5rCUzs1pQkyiFVKI4Bbj3XTuI81d8lbACuBBIQvwe%2FiRhDHmPtIwW%2F2vxLBw9I9%2FH53TcEuQNq6R6xCbOlX%2F9H1JvLn6OHO2X%2FlIOUZNNe7NBajkRZ%2FtAlHNJf1zYbvg9CvGh98%2FCH+D4gtSmzr1AsF%2FW1FGPfOw64oSHf0jlKnMwifg2h5q909mCgFRA=|tkp%3ABk9SR66a_urIZQ</t>
+  </si>
+  <si>
+    <t>240 W</t>
+  </si>
+  <si>
+    <t>7.4 V</t>
+  </si>
+  <si>
+    <t>SATYAS HOUSE</t>
+  </si>
+  <si>
+    <t>idk</t>
+  </si>
+  <si>
+    <t>FREEE</t>
+  </si>
   <si>
     <t>Quantity</t>
   </si>
@@ -55,10 +110,7 @@
     <t>Friction (N)</t>
   </si>
   <si>
-    <t>--&gt;</t>
-  </si>
-  <si>
-    <t>TARGET</t>
+    <t/>
   </si>
   <si>
     <t>dP/a</t>
@@ -69,7 +121,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,6 +130,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -86,6 +139,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -137,12 +196,36 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
@@ -151,32 +234,17 @@
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -512,47 +580,47 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="11" width="21.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="12" width="30.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="11" width="12.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="13" width="29.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="12" width="25.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="13" width="26.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="12" width="23.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="12" width="16.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="12" width="22.005" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="11" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="11" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="11" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="11" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="11" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="7" width="21.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="9" width="30.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="12.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="8" width="29.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="9" width="24.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="8" width="24.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="9" width="22.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="9" width="16.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="9" width="21.005" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="7" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="7" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="7" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="7" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="7" width="12.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>18</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>19</v>
       </c>
       <c r="C1" s="1"/>
-      <c r="D1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>7</v>
+      <c r="D1" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>25</v>
       </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -562,28 +630,28 @@
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="5">
+        <v>26</v>
+      </c>
+      <c r="B2" s="13">
         <v>200</v>
       </c>
       <c r="C2" s="1"/>
-      <c r="D2" s="5">
+      <c r="D2" s="13">
         <v>0</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="10">
         <f>D2 * 3.6</f>
       </c>
-      <c r="F2" s="5">
-        <f>D2/12 *300</f>
-      </c>
-      <c r="G2" s="2">
+      <c r="F2" s="13">
+        <f>D2/$B$4*$B$2</f>
+      </c>
+      <c r="G2" s="10">
         <f>(F2+$B$6)*$B$3</f>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="13">
         <f>60*D2/2*PI()*$B$3</f>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="13">
         <f>G2*H2*PI()/30</f>
       </c>
       <c r="J2" s="1"/>
@@ -594,28 +662,28 @@
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="2">
+        <v>27</v>
+      </c>
+      <c r="B3" s="10">
         <v>0.25</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="5">
+      <c r="D3" s="13">
         <f>D2+1</f>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="10">
         <f>D3 * 3.6</f>
       </c>
-      <c r="F3" s="5">
-        <f>D3/12 *300</f>
-      </c>
-      <c r="G3" s="2">
+      <c r="F3" s="13">
+        <f>D3/$B$4*$B$2</f>
+      </c>
+      <c r="G3" s="10">
         <f>(F3+$B$6)*$B$3</f>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="10">
         <f>60*D3/2*PI()*$B$3</f>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="10">
         <f>G3*H3*PI()/30</f>
       </c>
       <c r="J3" s="1"/>
@@ -626,28 +694,28 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="5">
+        <v>28</v>
+      </c>
+      <c r="B4" s="13">
         <v>12</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="5">
+      <c r="D4" s="13">
         <f>D3+1</f>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="10">
         <f>D4 * 3.6</f>
       </c>
-      <c r="F4" s="5">
-        <f>D4/12 *300</f>
-      </c>
-      <c r="G4" s="2">
+      <c r="F4" s="13">
+        <f>D4/$B$4*$B$2</f>
+      </c>
+      <c r="G4" s="10">
         <f>(F4+$B$6)*$B$3</f>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="10">
         <f>60*D4/2*PI()*$B$3</f>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="10">
         <f>G4*H4*PI()/30</f>
       </c>
       <c r="J4" s="1"/>
@@ -658,28 +726,28 @@
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="2">
+        <v>29</v>
+      </c>
+      <c r="B5" s="10">
         <v>0.012</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="5">
+      <c r="D5" s="13">
         <f>D4+1</f>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="10">
         <f>D5 * 3.6</f>
       </c>
-      <c r="F5" s="5">
-        <f>D5/12 *300</f>
-      </c>
-      <c r="G5" s="2">
+      <c r="F5" s="13">
+        <f>D5/$B$4*$B$2</f>
+      </c>
+      <c r="G5" s="10">
         <f>(F5+$B$6)*$B$3</f>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="10">
         <f>60*D5/2*PI()*$B$3</f>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="10">
         <f>G5*H5*PI()/30</f>
       </c>
       <c r="J5" s="1"/>
@@ -690,28 +758,28 @@
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="2">
+        <v>30</v>
+      </c>
+      <c r="B6" s="10">
         <f>B2*9.81*B5</f>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="5">
+      <c r="D6" s="13">
         <f>D5+1</f>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="10">
         <f>D6 * 3.6</f>
       </c>
-      <c r="F6" s="5">
-        <f>D6/12 *300</f>
-      </c>
-      <c r="G6" s="2">
+      <c r="F6" s="13">
+        <f>D6/$B$4*$B$2</f>
+      </c>
+      <c r="G6" s="10">
         <f>(F6+$B$6)*$B$3</f>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="10">
         <f>60*D6/2*PI()*$B$3</f>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="10">
         <f>G6*H6*PI()/30</f>
       </c>
       <c r="J6" s="1"/>
@@ -722,24 +790,24 @@
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="1"/>
-      <c r="B7" s="6"/>
+      <c r="B7" s="3"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="5">
+      <c r="D7" s="13">
         <f>D6+1</f>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="10">
         <f>D7 * 3.6</f>
       </c>
-      <c r="F7" s="5">
-        <f>D7/12 *300</f>
-      </c>
-      <c r="G7" s="2">
+      <c r="F7" s="13">
+        <f>D7/$B$4*$B$2</f>
+      </c>
+      <c r="G7" s="10">
         <f>(F7+$B$6)*$B$3</f>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="10">
         <f>60*D7/2*PI()*$B$3</f>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="10">
         <f>G7*H7*PI()/30</f>
       </c>
       <c r="J7" s="1"/>
@@ -750,24 +818,26 @@
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="1"/>
-      <c r="B8" s="6"/>
+      <c r="B8" s="14" t="s">
+        <v>31</v>
+      </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="5">
+      <c r="D8" s="13">
         <f>D7+1</f>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="10">
         <f>D8 * 3.6</f>
       </c>
-      <c r="F8" s="5">
-        <f>D8/12 *300</f>
-      </c>
-      <c r="G8" s="2">
+      <c r="F8" s="13">
+        <f>D8/$B$4*$B$2</f>
+      </c>
+      <c r="G8" s="10">
         <f>(F8+$B$6)*$B$3</f>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="10">
         <f>60*D8/2*PI()*$B$3</f>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="10">
         <f>G8*H8*PI()/30</f>
       </c>
       <c r="J8" s="1"/>
@@ -778,24 +848,24 @@
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="1"/>
-      <c r="B9" s="6"/>
+      <c r="B9" s="3"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="5">
+      <c r="D9" s="13">
         <f>D8+1</f>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="10">
         <f>D9 * 3.6</f>
       </c>
-      <c r="F9" s="5">
-        <f>D9/12 *300</f>
-      </c>
-      <c r="G9" s="2">
+      <c r="F9" s="13">
+        <f>D9/$B$4*$B$2</f>
+      </c>
+      <c r="G9" s="10">
         <f>(F9+$B$6)*$B$3</f>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="10">
         <f>60*D9/2*PI()*$B$3</f>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="10">
         <f>G9*H9</f>
       </c>
       <c r="J9" s="1"/>
@@ -806,24 +876,24 @@
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="1"/>
-      <c r="B10" s="6"/>
+      <c r="B10" s="3"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="5">
+      <c r="D10" s="13">
         <f>D9+1</f>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="10">
         <f>D10 * 3.6</f>
       </c>
-      <c r="F10" s="5">
-        <f>D10/12 *300</f>
-      </c>
-      <c r="G10" s="2">
+      <c r="F10" s="13">
+        <f>D10/$B$4*$B$2</f>
+      </c>
+      <c r="G10" s="10">
         <f>(F10+$B$6)*$B$3</f>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="10">
         <f>60*D10/2*PI()*$B$3</f>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="10">
         <f>G10*H10*PI()/30</f>
       </c>
       <c r="J10" s="1"/>
@@ -834,24 +904,24 @@
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="1"/>
-      <c r="B11" s="6"/>
+      <c r="B11" s="3"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="5">
+      <c r="D11" s="13">
         <f>D10+1</f>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="10">
         <f>D11 * 3.6</f>
       </c>
-      <c r="F11" s="5">
-        <f>D11/12 *300</f>
-      </c>
-      <c r="G11" s="2">
+      <c r="F11" s="13">
+        <f>D11/$B$4*$B$2</f>
+      </c>
+      <c r="G11" s="10">
         <f>(F11+$B$6)*$B$3</f>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="10">
         <f>60*D11/2*PI()*$B$3</f>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="10">
         <f>G11*H11*PI()/30</f>
       </c>
       <c r="J11" s="1"/>
@@ -862,26 +932,24 @@
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="1"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="8">
+      <c r="B12" s="3"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="15">
         <f>D11+1</f>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="16">
         <f>D12 * 3.6</f>
       </c>
-      <c r="F12" s="8">
-        <f>D12/12 *300</f>
-      </c>
-      <c r="G12" s="9">
+      <c r="F12" s="15">
+        <f>D12/$B$4*$B$2</f>
+      </c>
+      <c r="G12" s="16">
         <f>(F12+$B$6)*$B$3</f>
       </c>
-      <c r="H12" s="9">
+      <c r="H12" s="16">
         <f>60*D12/2*PI()*$B$3</f>
       </c>
-      <c r="I12" s="9">
+      <c r="I12" s="16">
         <f>G12*H12*PI()/30</f>
       </c>
       <c r="J12" s="1"/>
@@ -892,24 +960,24 @@
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="1"/>
-      <c r="B13" s="6"/>
+      <c r="B13" s="3"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="5">
+      <c r="D13" s="13">
         <f>D12+1</f>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="10">
         <f>D13 * 3.6</f>
       </c>
-      <c r="F13" s="5">
-        <f>D13/12 *300</f>
-      </c>
-      <c r="G13" s="2">
+      <c r="F13" s="13">
+        <f>D13/$B$4*$B$2</f>
+      </c>
+      <c r="G13" s="10">
         <f>(F13+$B$6)*$B$3</f>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="10">
         <f>60*D13/2*PI()*$B$3</f>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="10">
         <f>G13*H13*PI()/30</f>
       </c>
       <c r="J13" s="1"/>
@@ -920,24 +988,24 @@
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="1"/>
-      <c r="B14" s="6"/>
+      <c r="B14" s="3"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="5">
+      <c r="D14" s="13">
         <f>D13+1</f>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="10">
         <f>D14 * 3.6</f>
       </c>
-      <c r="F14" s="5">
-        <f>D14/12 *300</f>
-      </c>
-      <c r="G14" s="2">
+      <c r="F14" s="13">
+        <f>D14/$B$4*$B$2</f>
+      </c>
+      <c r="G14" s="10">
         <f>(F14+$B$6)*$B$3</f>
       </c>
-      <c r="H14" s="2">
+      <c r="H14" s="10">
         <f>60*D14/2*PI()*$B$3</f>
       </c>
-      <c r="I14" s="2">
+      <c r="I14" s="10">
         <f>G14*H14*PI()/30</f>
       </c>
       <c r="J14" s="1"/>
@@ -948,24 +1016,24 @@
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="1"/>
-      <c r="B15" s="6"/>
+      <c r="B15" s="3"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="5">
+      <c r="D15" s="13">
         <f>D14+1</f>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="10">
         <f>D15 * 3.6</f>
       </c>
-      <c r="F15" s="5">
-        <f>D15/12 *300</f>
-      </c>
-      <c r="G15" s="2">
+      <c r="F15" s="13">
+        <f>D15/$B$4*$B$2</f>
+      </c>
+      <c r="G15" s="10">
         <f>(F15+$B$6)*$B$3</f>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="10">
         <f>60*D15/2*PI()*$B$3</f>
       </c>
-      <c r="I15" s="2">
+      <c r="I15" s="10">
         <f>G15*H15*PI()/30</f>
       </c>
       <c r="J15" s="1"/>
@@ -976,24 +1044,24 @@
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="1"/>
-      <c r="B16" s="6"/>
+      <c r="B16" s="3"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="5">
+      <c r="D16" s="13">
         <f>D15+1</f>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="10">
         <f>D16 * 3.6</f>
       </c>
-      <c r="F16" s="5">
-        <f>D16/12 *300</f>
-      </c>
-      <c r="G16" s="2">
+      <c r="F16" s="13">
+        <f>D16/$B$4*$B$2</f>
+      </c>
+      <c r="G16" s="10">
         <f>(F16+$B$6)*$B$3</f>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="10">
         <f>60*D16/2*PI()*$B$3</f>
       </c>
-      <c r="I16" s="2">
+      <c r="I16" s="10">
         <f>G16*H16*PI()/30</f>
       </c>
       <c r="J16" s="1"/>
@@ -1004,24 +1072,24 @@
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="1"/>
-      <c r="B17" s="6"/>
+      <c r="B17" s="3"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="5">
+      <c r="D17" s="13">
         <f>D16+1</f>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="10">
         <f>D17 * 3.6</f>
       </c>
-      <c r="F17" s="5">
-        <f>D17/12 *300</f>
-      </c>
-      <c r="G17" s="2">
+      <c r="F17" s="13">
+        <f>D17/$B$4*$B$2</f>
+      </c>
+      <c r="G17" s="10">
         <f>(F17+$B$6)*$B$3</f>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="10">
         <f>60*D17/2*PI()*$B$3</f>
       </c>
-      <c r="I17" s="2">
+      <c r="I17" s="10">
         <f>G17*H17*PI()/30</f>
       </c>
       <c r="J17" s="1"/>
@@ -1032,24 +1100,24 @@
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="1"/>
-      <c r="B18" s="6"/>
+      <c r="B18" s="3"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="5">
+      <c r="D18" s="13">
         <f>D17+1</f>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="10">
         <f>D18 * 3.6</f>
       </c>
-      <c r="F18" s="5">
-        <f>D18/12 *300</f>
-      </c>
-      <c r="G18" s="2">
+      <c r="F18" s="13">
+        <f>D18/$B$4*$B$2</f>
+      </c>
+      <c r="G18" s="10">
         <f>(F18+$B$6)*$B$3</f>
       </c>
-      <c r="H18" s="2">
+      <c r="H18" s="10">
         <f>60*D18/2*PI()*$B$3</f>
       </c>
-      <c r="I18" s="2">
+      <c r="I18" s="10">
         <f>G18*H18*PI()/30</f>
       </c>
       <c r="J18" s="1"/>
@@ -1060,24 +1128,24 @@
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="1"/>
-      <c r="B19" s="6"/>
+      <c r="B19" s="3"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="5">
+      <c r="D19" s="13">
         <f>D18+1</f>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="10">
         <f>D19 * 3.6</f>
       </c>
-      <c r="F19" s="5">
-        <f>D19/12 *300</f>
-      </c>
-      <c r="G19" s="2">
+      <c r="F19" s="13">
+        <f>D19/$B$4*$B$2</f>
+      </c>
+      <c r="G19" s="10">
         <f>(F19+$B$6)*$B$3</f>
       </c>
-      <c r="H19" s="2">
+      <c r="H19" s="10">
         <f>60*D19/2*PI()*$B$3</f>
       </c>
-      <c r="I19" s="2">
+      <c r="I19" s="10">
         <f>G19*H19*PI()/30</f>
       </c>
       <c r="J19" s="1"/>
@@ -1088,24 +1156,24 @@
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="1"/>
-      <c r="B20" s="6"/>
+      <c r="B20" s="3"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="5">
+      <c r="D20" s="13">
         <f>D19+1</f>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="10">
         <f>D20 * 3.6</f>
       </c>
-      <c r="F20" s="5">
-        <f>D20/12 *300</f>
-      </c>
-      <c r="G20" s="2">
+      <c r="F20" s="13">
+        <f>D20/$B$4*$B$2</f>
+      </c>
+      <c r="G20" s="10">
         <f>(F20+$B$6)*$B$3</f>
       </c>
-      <c r="H20" s="2">
+      <c r="H20" s="10">
         <f>60*D20/2*PI()*$B$3</f>
       </c>
-      <c r="I20" s="2">
+      <c r="I20" s="10">
         <f>G20*H20*PI()/30</f>
       </c>
       <c r="J20" s="1"/>
@@ -1116,24 +1184,24 @@
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="1"/>
-      <c r="B21" s="6"/>
+      <c r="B21" s="3"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="5">
+      <c r="D21" s="13">
         <f>D20+1</f>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="10">
         <f>D21 * 3.6</f>
       </c>
-      <c r="F21" s="5">
-        <f>D21/12 *300</f>
-      </c>
-      <c r="G21" s="2">
+      <c r="F21" s="13">
+        <f>D21/$B$4*$B$2</f>
+      </c>
+      <c r="G21" s="10">
         <f>(F21+$B$6)*$B$3</f>
       </c>
-      <c r="H21" s="2">
+      <c r="H21" s="10">
         <f>60*D21/2*PI()*$B$3</f>
       </c>
-      <c r="I21" s="2">
+      <c r="I21" s="10">
         <f>G21*H21*PI()/30</f>
       </c>
       <c r="J21" s="1"/>
@@ -1144,24 +1212,24 @@
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="1"/>
-      <c r="B22" s="6"/>
+      <c r="B22" s="3"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="5">
+      <c r="D22" s="13">
         <f>D21+1</f>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="10">
         <f>D22 * 3.6</f>
       </c>
-      <c r="F22" s="5">
-        <f>D22/12 *300</f>
-      </c>
-      <c r="G22" s="2">
+      <c r="F22" s="13">
+        <f>D22/$B$4*$B$2</f>
+      </c>
+      <c r="G22" s="10">
         <f>(F22+$B$6)*$B$3</f>
       </c>
-      <c r="H22" s="2">
+      <c r="H22" s="10">
         <f>60*D22/2*PI()*$B$3</f>
       </c>
-      <c r="I22" s="2">
+      <c r="I22" s="10">
         <f>G22*H22*PI()/30</f>
       </c>
       <c r="J22" s="1"/>
@@ -1172,14 +1240,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="6"/>
+      <c r="B23" s="3"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
@@ -1188,16 +1256,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
       <c r="A24" s="1"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D24" s="10"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
@@ -1206,14 +1272,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
       <c r="A25" s="1"/>
-      <c r="B25" s="6"/>
+      <c r="B25" s="3"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
@@ -1222,14 +1288,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
       <c r="A26" s="1"/>
-      <c r="B26" s="6"/>
+      <c r="B26" s="3"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
@@ -1238,14 +1304,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
       <c r="A27" s="1"/>
-      <c r="B27" s="6"/>
+      <c r="B27" s="3"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
@@ -1254,14 +1320,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25">
       <c r="A28" s="1"/>
-      <c r="B28" s="6"/>
+      <c r="B28" s="3"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
@@ -1270,14 +1336,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25">
       <c r="A29" s="1"/>
-      <c r="B29" s="6"/>
+      <c r="B29" s="3"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
@@ -1286,14 +1352,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25">
       <c r="A30" s="1"/>
-      <c r="B30" s="6"/>
+      <c r="B30" s="3"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
@@ -1302,14 +1368,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25">
       <c r="A31" s="1"/>
-      <c r="B31" s="6"/>
+      <c r="B31" s="3"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
@@ -1318,14 +1384,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25">
       <c r="A32" s="1"/>
-      <c r="B32" s="6"/>
+      <c r="B32" s="3"/>
       <c r="C32" s="1"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
@@ -1334,14 +1400,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="17.25">
       <c r="A33" s="1"/>
-      <c r="B33" s="6"/>
+      <c r="B33" s="3"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
@@ -1350,14 +1416,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25">
       <c r="A34" s="1"/>
-      <c r="B34" s="6"/>
+      <c r="B34" s="3"/>
       <c r="C34" s="1"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
@@ -1366,14 +1432,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="17.25">
       <c r="A35" s="1"/>
-      <c r="B35" s="6"/>
+      <c r="B35" s="3"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="10"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="6"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
@@ -1382,14 +1448,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="17.25">
       <c r="A36" s="1"/>
-      <c r="B36" s="6"/>
+      <c r="B36" s="3"/>
       <c r="C36" s="1"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
@@ -1398,14 +1464,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="17.25">
       <c r="A37" s="1"/>
-      <c r="B37" s="6"/>
+      <c r="B37" s="3"/>
       <c r="C37" s="1"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
@@ -1414,20 +1480,20 @@
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="17.25">
       <c r="A38" s="1"/>
-      <c r="B38" s="6"/>
+      <c r="B38" s="3"/>
       <c r="C38" s="1"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="6"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
       <c r="N38" s="1" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1437,4 +1503,135 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="7" width="43.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="30.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="8" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="9" width="12.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+  </cols>
+  <sheetData>
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="166">
+      <c r="A3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="176">
+      <c r="A4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="5">
+        <v>21000</v>
+      </c>
+      <c r="F4" s="6">
+        <f>(9550*0.24)/E4</f>
+      </c>
+      <c r="G4" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
gear ratio table is almost finished, satya will finish it ig
</commit_message>
<xml_diff>
--- a/Motor_calculations/Car calculations.xlsx
+++ b/Motor_calculations/Car calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ronitbhandari/Desktop/VELOX/Motor_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1545C8D-FCA2-E748-82C0-358B1BFFBCC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1B04A6A-DF48-DA4F-B0A0-A3975E9336C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,8 +32,64 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Ronit Bhandari</author>
+  </authors>
+  <commentList>
+    <comment ref="J22" authorId="0" shapeId="0" xr:uid="{7BEA248F-B2AE-5241-843D-678136970A79}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ronit Bhandari:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t>Quantity</t>
   </si>
@@ -60,9 +116,6 @@
   </si>
   <si>
     <t>mass (kg)</t>
-  </si>
-  <si>
-    <t>radius (m)</t>
   </si>
   <si>
     <t>time to reach velocity (s)</t>
@@ -141,6 +194,21 @@
   <si>
     <t>Calculated Torque</t>
   </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>*pi</t>
+  </si>
+  <si>
+    <t>/30</t>
+  </si>
+  <si>
+    <t>Closes Power Rating</t>
+  </si>
+  <si>
+    <t>tire radius (m)</t>
+  </si>
 </sst>
 </file>
 
@@ -149,7 +217,7 @@
   <numFmts count="1">
     <numFmt numFmtId="168" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -185,6 +253,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -358,11 +439,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -376,7 +455,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -412,7 +490,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -746,14 +827,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:R38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" zoomScale="84" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -840,7 +921,7 @@
     </row>
     <row r="3" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="B3" s="1">
         <v>0.25</v>
@@ -876,7 +957,7 @@
     </row>
     <row r="4" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="4">
         <v>12</v>
@@ -912,7 +993,7 @@
     </row>
     <row r="5" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1">
         <v>1.2E-2</v>
@@ -948,7 +1029,7 @@
     </row>
     <row r="6" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1">
         <f>B2*9.81*B5</f>
@@ -1062,14 +1143,14 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
+      <c r="A10" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="43"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="17"/>
       <c r="H10" s="4">
         <f t="shared" si="5"/>
         <v>8</v>
@@ -1096,15 +1177,15 @@
       </c>
     </row>
     <row r="11" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="39"/>
-      <c r="C11" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="38"/>
-      <c r="E11" s="39"/>
+      <c r="A11" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="38"/>
+      <c r="C11" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="37"/>
+      <c r="E11" s="38"/>
       <c r="F11" s="18"/>
       <c r="H11" s="4">
         <f t="shared" si="5"/>
@@ -1132,14 +1213,18 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="21"/>
-      <c r="B12" s="35"/>
+      <c r="A12" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="29">
+        <v>1500</v>
+      </c>
       <c r="C12" s="21"/>
       <c r="D12" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="34" t="s">
         <v>27</v>
-      </c>
-      <c r="E12" s="35" t="s">
-        <v>28</v>
       </c>
       <c r="H12" s="7">
         <f>H11+1</f>
@@ -1170,14 +1255,14 @@
       <c r="A13" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="30">
-        <v>1800</v>
+      <c r="B13" s="29">
+        <v>2000</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D13" s="9"/>
-      <c r="E13" s="34"/>
+      <c r="E13" s="33"/>
       <c r="G13" s="6"/>
       <c r="H13" s="4">
         <f>H12+1</f>
@@ -1205,17 +1290,18 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="30">
-        <v>4500</v>
+      <c r="A14" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="29">
+        <f>B12*30/B13*PI()</f>
+        <v>70.685834705770347</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D14" s="9"/>
-      <c r="E14" s="33"/>
+      <c r="E14" s="32"/>
       <c r="H14" s="4">
         <f>H13+1</f>
         <v>12</v>
@@ -1242,17 +1328,14 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="30">
-        <f>B13*30/B14*PI()</f>
-        <v>37.699111843077517</v>
-      </c>
+      <c r="A15" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="35"/>
       <c r="C15" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15" s="30"/>
+        <v>28</v>
+      </c>
+      <c r="E15" s="29"/>
       <c r="H15" s="4">
         <f>H14+1</f>
         <v>13</v>
@@ -1279,15 +1362,18 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="36"/>
-      <c r="C16" s="26" t="s">
-        <v>23</v>
+      <c r="A16" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="29" cm="1">
+        <f t="array" ref="B16">INDEX(Table1[(REQUIRED) RPM],MATCH(MIN(ABS(Table1[(REQUIRED) Power (W)]- B12)), ABS(Table1[(REQUIRED) Power (W)]- B12), 0))</f>
+        <v>212.05750411731103</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>22</v>
       </c>
       <c r="D16" s="20"/>
-      <c r="E16" s="32"/>
+      <c r="E16" s="31"/>
       <c r="F16" s="19"/>
       <c r="H16" s="4">
         <f>H15+1</f>
@@ -1315,19 +1401,19 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="42" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="30">
-        <f>INDEX(Table1[(REQUIRED) RPM], MATCH(B13, Table1[(REQUIRED) Power (W)],1 ))</f>
-        <v>235.61944901923448</v>
-      </c>
-      <c r="C17" s="25"/>
-      <c r="D17" s="17" t="s">
+      <c r="A17" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="29" cm="1">
+        <f t="array" ref="B17">INDEX(Table1[(REQUIRED) Torque (Nm)],MATCH(MIN(ABS(Table1[(REQUIRED) Power (W)]- B12)), ABS(Table1[(REQUIRED) Power (W)]- B12), 0))</f>
+        <v>62.136000000000003</v>
+      </c>
+      <c r="C17" s="39"/>
+      <c r="D17" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="30" t="s">
         <v>24</v>
-      </c>
-      <c r="E17" s="31" t="s">
-        <v>25</v>
       </c>
       <c r="H17" s="4">
         <f>H16+1</f>
@@ -1355,18 +1441,18 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="43" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="29">
-        <f>INDEX(Table1[(REQUIRED) Torque (Nm)], MATCH(B13, Table1[(REQUIRED) Power (W)],1 ))</f>
-        <v>68.385999999999996</v>
+      <c r="A18" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="28" cm="1">
+        <f t="array" ref="B18">INDEX(Table1[(REQUIRED) Power (W)],MATCH(MIN(ABS(Table1[(REQUIRED) Power (W)]- B12)), ABS(Table1[(REQUIRED) Power (W)]- B12), 0))</f>
+        <v>1379.8299128986987</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D18" s="12"/>
-      <c r="E18" s="30"/>
+      <c r="E18" s="29"/>
       <c r="H18" s="4">
         <f>H17+1</f>
         <v>16</v>
@@ -1394,11 +1480,11 @@
     </row>
     <row r="19" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="13"/>
-      <c r="C19" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="28"/>
-      <c r="E19" s="29"/>
+      <c r="C19" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="27"/>
+      <c r="E19" s="28"/>
       <c r="H19" s="4">
         <f>H18+1</f>
         <v>17</v>
@@ -1426,7 +1512,7 @@
     </row>
     <row r="20" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="13"/>
-      <c r="C20" s="40"/>
+      <c r="C20" s="39"/>
       <c r="H20" s="4">
         <f>H19+1</f>
         <v>18</v>
@@ -1479,7 +1565,11 @@
       </c>
     </row>
     <row r="22" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D22" s="16"/>
+      <c r="B22" s="5">
+        <f>B16*B17*PI()/30</f>
+        <v>1379.8299128986987</v>
+      </c>
+      <c r="D22" s="15"/>
       <c r="H22" s="4">
         <f>H21+1</f>
         <v>20</v>
@@ -1507,7 +1597,23 @@
     </row>
     <row r="23" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="24" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
     <row r="26" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="28" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="29" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1523,15 +1629,15 @@
     <row r="37" spans="18:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="38" spans="18:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R38" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="C16:E16"/>
+    <mergeCell ref="A15:B15"/>
     <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A10:E10"/>
     <mergeCell ref="C11:E11"/>
   </mergeCells>
   <conditionalFormatting sqref="A21">
@@ -1545,9 +1651,10 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
   <tableParts count="2">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Trouble shooting equations, also created a python script to calculate gear ratios to make sure everything being done is actually correct
</commit_message>
<xml_diff>
--- a/Motor_calculations/Car calculations.xlsx
+++ b/Motor_calculations/Car calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ronitbhandari/Desktop/VELOX/Motor_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1B04A6A-DF48-DA4F-B0A0-A3975E9336C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85A632B0-AB48-D349-95F2-DF04980CA407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
     <author>Ronit Bhandari</author>
   </authors>
   <commentList>
-    <comment ref="J22" authorId="0" shapeId="0" xr:uid="{7BEA248F-B2AE-5241-843D-678136970A79}">
+    <comment ref="K23" authorId="0" shapeId="0" xr:uid="{7BEA248F-B2AE-5241-843D-678136970A79}">
       <text>
         <r>
           <rPr>
@@ -367,34 +367,40 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -444,6 +450,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -476,22 +485,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -516,8 +522,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="H1:M22" totalsRowShown="0">
-  <autoFilter ref="H1:M22" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="I2:N23" totalsRowShown="0">
+  <autoFilter ref="I2:N23" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="velocity (m/s) (TARGET VALUE)"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="(REQUIRED) velocity (km/h)"/>
@@ -525,7 +531,7 @@
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="(REQUIRED) Torque (Nm)"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="(REQUIRED) RPM"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="(REQUIRED) Power (W)" dataDxfId="0">
-      <calculatedColumnFormula>K2*L2*PI()/30</calculatedColumnFormula>
+      <calculatedColumnFormula>L3*M3*PI()/30</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -533,8 +539,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:B6" totalsRowShown="0">
-  <autoFilter ref="A1:B6" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="B2:C7" totalsRowShown="0">
+  <autoFilter ref="B2:C7" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Quantity"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Value"/>
@@ -831,816 +837,816 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:R38"/>
+  <dimension ref="B2:S39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="113" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" customWidth="1"/>
-    <col min="2" max="2" width="22.5" style="5" customWidth="1"/>
-    <col min="3" max="6" width="12.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.1640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.83203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="89.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="22.5" style="5" customWidth="1"/>
+    <col min="4" max="7" width="12.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.1640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.83203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="89.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="2" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="H1" s="2" t="s">
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="I2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="J2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="N2" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="3" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="4">
+      <c r="C3" s="4">
         <v>200</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="H2" s="4">
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="I3" s="4">
         <v>0</v>
       </c>
-      <c r="I2" s="1">
-        <f t="shared" ref="I2:I11" si="0">H2 * 3.6</f>
+      <c r="J3" s="1">
+        <f t="shared" ref="J3:J12" si="0">I3 * 3.6</f>
         <v>0</v>
       </c>
-      <c r="J2" s="4">
-        <f t="shared" ref="J2:J11" si="1">H2/12 *300</f>
+      <c r="K3" s="4">
+        <f t="shared" ref="K3:K12" si="1">I3/12 *300</f>
         <v>0</v>
       </c>
-      <c r="K2" s="1">
-        <f t="shared" ref="K2:K11" si="2">(J2+$B$6)*$B$3</f>
+      <c r="L3" s="1">
+        <f t="shared" ref="L3:L12" si="2">(K3+$C$7)*$C$4</f>
         <v>5.8860000000000001</v>
       </c>
-      <c r="L2" s="4">
-        <f t="shared" ref="L2:L11" si="3">60*H2/2*PI()*$B$3</f>
+      <c r="M3" s="4">
+        <f t="shared" ref="M3:M12" si="3">60*I3/2*PI()*$C$4</f>
         <v>0</v>
       </c>
-      <c r="M2" s="1">
-        <f t="shared" ref="M2:M11" si="4">K2*L2*PI()/30</f>
+      <c r="N3" s="1">
+        <f t="shared" ref="N3:N12" si="4">L3*M3*PI()/30</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="4" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="1">
+      <c r="C4" s="1">
         <v>0.25</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="H3" s="4">
-        <f t="shared" ref="H3:H23" si="5">H2+1</f>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="I4" s="4">
+        <f t="shared" ref="I4:I24" si="5">I3+1</f>
         <v>1</v>
       </c>
-      <c r="I3" s="1">
+      <c r="J4" s="1">
         <f t="shared" si="0"/>
         <v>3.6</v>
       </c>
-      <c r="J3" s="4">
+      <c r="K4" s="4">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="K3" s="1">
+      <c r="L4" s="1">
         <f t="shared" si="2"/>
         <v>12.135999999999999</v>
       </c>
-      <c r="L3" s="1">
+      <c r="M4" s="1">
         <f t="shared" si="3"/>
         <v>23.561944901923447</v>
       </c>
-      <c r="M3" s="1">
+      <c r="N4" s="1">
         <f t="shared" si="4"/>
         <v>29.944379752905107</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="5" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4">
+      <c r="C5" s="4">
         <v>12</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="H4" s="4">
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="I5" s="4">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="I4" s="1">
+      <c r="J5" s="1">
         <f t="shared" si="0"/>
         <v>7.2</v>
       </c>
-      <c r="J4" s="4">
+      <c r="K5" s="4">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="K4" s="1">
+      <c r="L5" s="1">
         <f t="shared" si="2"/>
         <v>18.385999999999999</v>
       </c>
-      <c r="L4" s="1">
+      <c r="M5" s="1">
         <f t="shared" si="3"/>
         <v>47.123889803846893</v>
       </c>
-      <c r="M4" s="1">
+      <c r="N5" s="1">
         <f t="shared" si="4"/>
         <v>90.731273259214461</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="6" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="1">
+      <c r="C6" s="1">
         <v>1.2E-2</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="H5" s="4">
-        <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
-      <c r="I5" s="1">
-        <f t="shared" si="0"/>
-        <v>10.8</v>
-      </c>
-      <c r="J5" s="4">
-        <f t="shared" si="1"/>
-        <v>75</v>
-      </c>
-      <c r="K5" s="1">
-        <f t="shared" si="2"/>
-        <v>24.635999999999999</v>
-      </c>
-      <c r="L5" s="1">
-        <f t="shared" si="3"/>
-        <v>70.685834705770347</v>
-      </c>
-      <c r="M5" s="1">
-        <f t="shared" si="4"/>
-        <v>182.36068051892804</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1">
-        <f>B2*9.81*B5</f>
-        <v>23.544</v>
-      </c>
-      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="H6" s="4">
+      <c r="G6" s="1"/>
+      <c r="I6" s="4">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="J6" s="1">
+        <f t="shared" si="0"/>
+        <v>10.8</v>
+      </c>
+      <c r="K6" s="4">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="L6" s="1">
+        <f t="shared" si="2"/>
+        <v>24.635999999999999</v>
+      </c>
+      <c r="M6" s="1">
+        <f t="shared" si="3"/>
+        <v>70.685834705770347</v>
+      </c>
+      <c r="N6" s="1">
+        <f t="shared" si="4"/>
+        <v>182.36068051892804</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1">
+        <f>C3*9.81*C6</f>
+        <v>23.544</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="I7" s="4">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="I6" s="1">
+      <c r="J7" s="1">
         <f t="shared" si="0"/>
         <v>14.4</v>
       </c>
-      <c r="J6" s="4">
+      <c r="K7" s="4">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="K6" s="1">
+      <c r="L7" s="1">
         <f t="shared" si="2"/>
         <v>30.885999999999999</v>
       </c>
-      <c r="L6" s="1">
+      <c r="M7" s="1">
         <f t="shared" si="3"/>
         <v>94.247779607693786</v>
       </c>
-      <c r="M6" s="1">
+      <c r="N7" s="1">
         <f t="shared" si="4"/>
         <v>304.83260153204589</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H7" s="4">
+    <row r="8" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I8" s="4">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
-      <c r="I7" s="1">
+      <c r="J8" s="1">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="J7" s="4">
+      <c r="K8" s="4">
         <f t="shared" si="1"/>
         <v>125</v>
       </c>
-      <c r="K7" s="1">
+      <c r="L8" s="1">
         <f t="shared" si="2"/>
         <v>37.136000000000003</v>
       </c>
-      <c r="L7" s="1">
+      <c r="M8" s="1">
         <f t="shared" si="3"/>
         <v>117.80972450961724</v>
       </c>
-      <c r="M7" s="1">
+      <c r="N8" s="1">
         <f t="shared" si="4"/>
         <v>458.14703629856803</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H8" s="4">
+    <row r="9" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I9" s="4">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
-      <c r="I8" s="1">
+      <c r="J9" s="1">
         <f t="shared" si="0"/>
         <v>21.6</v>
       </c>
-      <c r="J8" s="4">
+      <c r="K9" s="4">
         <f t="shared" si="1"/>
         <v>150</v>
       </c>
-      <c r="K8" s="1">
+      <c r="L9" s="1">
         <f t="shared" si="2"/>
         <v>43.386000000000003</v>
       </c>
-      <c r="L8" s="1">
+      <c r="M9" s="1">
         <f t="shared" si="3"/>
         <v>141.37166941154069</v>
       </c>
-      <c r="M8" s="1">
+      <c r="N9" s="1">
         <f t="shared" si="4"/>
         <v>642.30398481849443</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H9" s="4">
+    <row r="10" spans="2:14" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I10" s="4">
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
-      <c r="I9" s="1">
+      <c r="J10" s="1">
         <f t="shared" si="0"/>
         <v>25.2</v>
       </c>
-      <c r="J9" s="4">
+      <c r="K10" s="4">
         <f t="shared" si="1"/>
         <v>175</v>
       </c>
-      <c r="K9" s="1">
+      <c r="L10" s="1">
         <f t="shared" si="2"/>
         <v>49.636000000000003</v>
       </c>
-      <c r="L9" s="1">
+      <c r="M10" s="1">
         <f t="shared" si="3"/>
         <v>164.93361431346415</v>
       </c>
-      <c r="M9" s="1">
+      <c r="N10" s="1">
         <f t="shared" si="4"/>
         <v>857.30344709182498</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="43" t="s">
+    <row r="11" spans="2:14" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="43"/>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="17"/>
-      <c r="H10" s="4">
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="17"/>
+      <c r="I11" s="4">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="I10" s="1">
+      <c r="J11" s="1">
         <f t="shared" si="0"/>
         <v>28.8</v>
       </c>
-      <c r="J10" s="4">
+      <c r="K11" s="4">
         <f t="shared" si="1"/>
         <v>200</v>
       </c>
-      <c r="K10" s="1">
+      <c r="L11" s="1">
         <f t="shared" si="2"/>
         <v>55.886000000000003</v>
       </c>
-      <c r="L10" s="1">
+      <c r="M11" s="1">
         <f t="shared" si="3"/>
         <v>188.49555921538757</v>
       </c>
-      <c r="M10" s="1">
+      <c r="N11" s="1">
         <f t="shared" si="4"/>
         <v>1103.1454231185596</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="36" t="s">
+    <row r="12" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="38"/>
-      <c r="C11" s="36" t="s">
+      <c r="C12" s="36"/>
+      <c r="D12" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="37"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="18"/>
-      <c r="H11" s="4">
+      <c r="E12" s="20"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="18"/>
+      <c r="I12" s="4">
         <f t="shared" si="5"/>
         <v>9</v>
       </c>
-      <c r="I11" s="1">
+      <c r="J12" s="1">
         <f t="shared" si="0"/>
         <v>32.4</v>
       </c>
-      <c r="J11" s="4">
+      <c r="K12" s="4">
         <f t="shared" si="1"/>
         <v>225</v>
       </c>
-      <c r="K11" s="1">
+      <c r="L12" s="1">
         <f t="shared" si="2"/>
         <v>62.136000000000003</v>
       </c>
-      <c r="L11" s="1">
+      <c r="M12" s="1">
         <f t="shared" si="3"/>
         <v>212.05750411731103</v>
       </c>
-      <c r="M11" s="1">
+      <c r="N12" s="1">
         <f t="shared" si="4"/>
         <v>1379.8299128986987</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="40" t="s">
+    <row r="13" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="29">
-        <v>1500</v>
-      </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="14" t="s">
+      <c r="C13" s="30">
+        <v>1687.36</v>
+      </c>
+      <c r="D13" s="22"/>
+      <c r="E13" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="34" t="s">
+      <c r="F13" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="7">
-        <f>H11+1</f>
+      <c r="I13" s="7">
+        <f>I12+1</f>
         <v>10</v>
       </c>
-      <c r="I12" s="8">
-        <f>H12 * 3.6</f>
+      <c r="J13" s="8">
+        <f>I13 * 3.6</f>
         <v>36</v>
       </c>
-      <c r="J12" s="7">
-        <f>H12/12 *300</f>
+      <c r="K13" s="7">
+        <f>I13/12 *300</f>
         <v>250</v>
       </c>
-      <c r="K12" s="8">
-        <f>(J12+$B$6)*$B$3</f>
+      <c r="L13" s="8">
+        <f>(K13+$C$7)*$C$4</f>
         <v>68.385999999999996</v>
       </c>
-      <c r="L12" s="8">
-        <f>60*H12/2*PI()*$B$3</f>
+      <c r="M13" s="8">
+        <f>60*I13/2*PI()*$C$4</f>
         <v>235.61944901923448</v>
       </c>
-      <c r="M12" s="1">
-        <f>K12*L12*PI()/30</f>
+      <c r="N13" s="1">
+        <f>L13*M13*PI()/30</f>
         <v>1687.3569164322421</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="41" t="s">
+    <row r="14" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="29">
+      <c r="C14" s="30">
         <v>2000</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="D14" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="33"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="4">
-        <f>H12+1</f>
+      <c r="E14" s="9"/>
+      <c r="F14" s="34"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="4">
+        <f>I13+1</f>
         <v>11</v>
       </c>
-      <c r="I13" s="1">
-        <f>H13 * 3.6</f>
+      <c r="J14" s="1">
+        <f>I14 * 3.6</f>
         <v>39.6</v>
       </c>
-      <c r="J13" s="4">
-        <f>H13/12 *300</f>
+      <c r="K14" s="4">
+        <f>I14/12 *300</f>
         <v>275</v>
       </c>
-      <c r="K13" s="1">
-        <f>(J13+$B$6)*$B$3</f>
+      <c r="L14" s="1">
+        <f>(K14+$C$7)*$C$4</f>
         <v>74.635999999999996</v>
       </c>
-      <c r="L13" s="1">
-        <f>60*H13/2*PI()*$B$3</f>
+      <c r="M14" s="1">
+        <f>60*I14/2*PI()*$C$4</f>
         <v>259.18139392115791</v>
       </c>
-      <c r="M13" s="1">
-        <f>K13*L13*PI()/30</f>
+      <c r="N14" s="1">
+        <f>L14*M14*PI()/30</f>
         <v>2025.7264337191891</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="41" t="s">
+    <row r="15" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="29">
-        <f>B12*30/B13*PI()</f>
-        <v>70.685834705770347</v>
-      </c>
-      <c r="C14" s="23" t="s">
+      <c r="C15" s="30">
+        <f>9550*C13/C14</f>
+        <v>8057.1439999999993</v>
+      </c>
+      <c r="D15" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="32"/>
-      <c r="H14" s="4">
-        <f>H13+1</f>
+      <c r="E15" s="9"/>
+      <c r="F15" s="33"/>
+      <c r="I15" s="4">
+        <f>I14+1</f>
         <v>12</v>
       </c>
-      <c r="I14" s="1">
-        <f>H14 * 3.6</f>
+      <c r="J15" s="1">
+        <f>I15 * 3.6</f>
         <v>43.2</v>
       </c>
-      <c r="J14" s="4">
-        <f>H14/12 *300</f>
+      <c r="K15" s="4">
+        <f>I15/12 *300</f>
         <v>300</v>
       </c>
-      <c r="K14" s="1">
-        <f>(J14+$B$6)*$B$3</f>
+      <c r="L15" s="1">
+        <f>(K15+$C$7)*$C$4</f>
         <v>80.885999999999996</v>
       </c>
-      <c r="L14" s="1">
-        <f>60*H14/2*PI()*$B$3</f>
+      <c r="M15" s="1">
+        <f>60*I15/2*PI()*$C$4</f>
         <v>282.74333882308139</v>
       </c>
-      <c r="M14" s="1">
-        <f>K14*L14*PI()/30</f>
+      <c r="N15" s="1">
+        <f>L15*M15*PI()/30</f>
         <v>2394.9384647595411</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="24" t="s">
+    <row r="16" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="35"/>
-      <c r="C15" s="23" t="s">
+      <c r="C16" s="36"/>
+      <c r="D16" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="29"/>
-      <c r="H15" s="4">
-        <f>H14+1</f>
+      <c r="F16" s="30"/>
+      <c r="I16" s="4">
+        <f>I15+1</f>
         <v>13</v>
       </c>
-      <c r="I15" s="1">
-        <f>H15 * 3.6</f>
+      <c r="J16" s="1">
+        <f>I16 * 3.6</f>
         <v>46.800000000000004</v>
       </c>
-      <c r="J15" s="4">
-        <f>H15/12 *300</f>
+      <c r="K16" s="4">
+        <f>I16/12 *300</f>
         <v>325</v>
       </c>
-      <c r="K15" s="1">
-        <f>(J15+$B$6)*$B$3</f>
+      <c r="L16" s="1">
+        <f>(K16+$C$7)*$C$4</f>
         <v>87.135999999999996</v>
       </c>
-      <c r="L15" s="1">
-        <f>60*H15/2*PI()*$B$3</f>
+      <c r="M16" s="1">
+        <f>60*I16/2*PI()*$C$4</f>
         <v>306.30528372500481</v>
       </c>
-      <c r="M15" s="1">
-        <f>K15*L15*PI()/30</f>
+      <c r="N16" s="1">
+        <f>L16*M16*PI()/30</f>
         <v>2794.9930095532973</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="41" t="s">
+    <row r="17" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="29" cm="1">
-        <f t="array" ref="B16">INDEX(Table1[(REQUIRED) RPM],MATCH(MIN(ABS(Table1[(REQUIRED) Power (W)]- B12)), ABS(Table1[(REQUIRED) Power (W)]- B12), 0))</f>
-        <v>212.05750411731103</v>
-      </c>
-      <c r="C16" s="25" t="s">
+      <c r="C17" s="30" cm="1">
+        <f t="array" ref="C17">INDEX(Table1[(REQUIRED) RPM],MATCH(MIN(ABS(Table1[(REQUIRED) Power (W)]- C13)), ABS(Table1[(REQUIRED) Power (W)]- C13), 0))</f>
+        <v>235.61944901923448</v>
+      </c>
+      <c r="D17" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="20"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="19"/>
-      <c r="H16" s="4">
-        <f>H15+1</f>
+      <c r="E17" s="21"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="19"/>
+      <c r="I17" s="4">
+        <f>I16+1</f>
         <v>14</v>
       </c>
-      <c r="I16" s="1">
-        <f>H16 * 3.6</f>
+      <c r="J17" s="1">
+        <f>I17 * 3.6</f>
         <v>50.4</v>
       </c>
-      <c r="J16" s="4">
-        <f>H16/12 *300</f>
+      <c r="K17" s="4">
+        <f>I17/12 *300</f>
         <v>350</v>
       </c>
-      <c r="K16" s="1">
-        <f>(J16+$B$6)*$B$3</f>
+      <c r="L17" s="1">
+        <f>(K17+$C$7)*$C$4</f>
         <v>93.385999999999996</v>
       </c>
-      <c r="L16" s="1">
-        <f>60*H16/2*PI()*$B$3</f>
+      <c r="M17" s="1">
+        <f>60*I17/2*PI()*$C$4</f>
         <v>329.86722862692829</v>
       </c>
-      <c r="M16" s="1">
-        <f>K16*L16*PI()/30</f>
+      <c r="N17" s="1">
+        <f>L17*M17*PI()/30</f>
         <v>3225.8900681004575</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="41" t="s">
+    <row r="18" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="29" cm="1">
-        <f t="array" ref="B17">INDEX(Table1[(REQUIRED) Torque (Nm)],MATCH(MIN(ABS(Table1[(REQUIRED) Power (W)]- B12)), ABS(Table1[(REQUIRED) Power (W)]- B12), 0))</f>
-        <v>62.136000000000003</v>
-      </c>
-      <c r="C17" s="39"/>
-      <c r="D17" s="16" t="s">
+      <c r="C18" s="30" cm="1">
+        <f t="array" ref="C18">INDEX(Table1[(REQUIRED) Torque (Nm)],MATCH(MIN(ABS(Table1[(REQUIRED) Power (W)]- C13)), ABS(Table1[(REQUIRED) Power (W)]- C13), 0))</f>
+        <v>68.385999999999996</v>
+      </c>
+      <c r="D18" s="37"/>
+      <c r="E18" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="30" t="s">
+      <c r="F18" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="H17" s="4">
-        <f>H16+1</f>
+      <c r="I18" s="4">
+        <f>I17+1</f>
         <v>15</v>
       </c>
-      <c r="I17" s="1">
-        <f>H17 * 3.6</f>
+      <c r="J18" s="1">
+        <f>I18 * 3.6</f>
         <v>54</v>
       </c>
-      <c r="J17" s="4">
-        <f>H17/12 *300</f>
+      <c r="K18" s="4">
+        <f>I18/12 *300</f>
         <v>375</v>
       </c>
-      <c r="K17" s="1">
-        <f>(J17+$B$6)*$B$3</f>
+      <c r="L18" s="1">
+        <f>(K18+$C$7)*$C$4</f>
         <v>99.635999999999996</v>
       </c>
-      <c r="L17" s="1">
-        <f>60*H17/2*PI()*$B$3</f>
+      <c r="M18" s="1">
+        <f>60*I18/2*PI()*$C$4</f>
         <v>353.42917352885172</v>
       </c>
-      <c r="M17" s="1">
-        <f>K17*L17*PI()/30</f>
+      <c r="N18" s="1">
+        <f>L18*M18*PI()/30</f>
         <v>3687.6296404010222</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="42" t="s">
+    <row r="19" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="28" cm="1">
-        <f t="array" ref="B18">INDEX(Table1[(REQUIRED) Power (W)],MATCH(MIN(ABS(Table1[(REQUIRED) Power (W)]- B12)), ABS(Table1[(REQUIRED) Power (W)]- B12), 0))</f>
-        <v>1379.8299128986987</v>
-      </c>
-      <c r="C18" s="23" t="s">
+      <c r="C19" s="29" cm="1">
+        <f t="array" ref="C19">INDEX(Table1[(REQUIRED) Power (W)],MATCH(MIN(ABS(Table1[(REQUIRED) Power (W)]- C13)), ABS(Table1[(REQUIRED) Power (W)]- C13), 0))</f>
+        <v>1687.3569164322421</v>
+      </c>
+      <c r="D19" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="12"/>
-      <c r="E18" s="29"/>
-      <c r="H18" s="4">
-        <f>H17+1</f>
+      <c r="E19" s="12"/>
+      <c r="F19" s="30"/>
+      <c r="I19" s="4">
+        <f>I18+1</f>
         <v>16</v>
       </c>
-      <c r="I18" s="1">
-        <f>H18 * 3.6</f>
+      <c r="J19" s="1">
+        <f>I19 * 3.6</f>
         <v>57.6</v>
       </c>
-      <c r="J18" s="4">
-        <f>H18/12 *300</f>
+      <c r="K19" s="4">
+        <f>I19/12 *300</f>
         <v>400</v>
       </c>
-      <c r="K18" s="1">
-        <f>(J18+$B$6)*$B$3</f>
+      <c r="L19" s="1">
+        <f>(K19+$C$7)*$C$4</f>
         <v>105.886</v>
       </c>
-      <c r="L18" s="1">
-        <f>60*H18/2*PI()*$B$3</f>
+      <c r="M19" s="1">
+        <f>60*I19/2*PI()*$C$4</f>
         <v>376.99111843077515</v>
       </c>
-      <c r="M18" s="1">
-        <f>K18*L18*PI()/30</f>
+      <c r="N19" s="1">
+        <f>L19*M19*PI()/30</f>
         <v>4180.2117264549906</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="13"/>
-      <c r="C19" s="26" t="s">
+    <row r="20" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="13"/>
+      <c r="D20" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="27"/>
-      <c r="E19" s="28"/>
-      <c r="H19" s="4">
-        <f>H18+1</f>
+      <c r="E20" s="28"/>
+      <c r="F20" s="29"/>
+      <c r="I20" s="4">
+        <f>I19+1</f>
         <v>17</v>
       </c>
-      <c r="I19" s="1">
-        <f>H19 * 3.6</f>
+      <c r="J20" s="1">
+        <f>I20 * 3.6</f>
         <v>61.2</v>
       </c>
-      <c r="J19" s="4">
-        <f>H19/12 *300</f>
+      <c r="K20" s="4">
+        <f>I20/12 *300</f>
         <v>425</v>
       </c>
-      <c r="K19" s="1">
-        <f>(J19+$B$6)*$B$3</f>
+      <c r="L20" s="1">
+        <f>(K20+$C$7)*$C$4</f>
         <v>112.136</v>
       </c>
-      <c r="L19" s="1">
-        <f>60*H19/2*PI()*$B$3</f>
+      <c r="M20" s="1">
+        <f>60*I20/2*PI()*$C$4</f>
         <v>400.55306333269863</v>
       </c>
-      <c r="M19" s="1">
-        <f>K19*L19*PI()/30</f>
+      <c r="N20" s="1">
+        <f>L20*M20*PI()/30</f>
         <v>4703.6363262623645</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="13"/>
-      <c r="C20" s="39"/>
-      <c r="H20" s="4">
-        <f>H19+1</f>
+    <row r="21" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="13"/>
+      <c r="D21" s="37"/>
+      <c r="I21" s="4">
+        <f>I20+1</f>
         <v>18</v>
       </c>
-      <c r="I20" s="1">
-        <f>H20 * 3.6</f>
+      <c r="J21" s="1">
+        <f>I21 * 3.6</f>
         <v>64.8</v>
       </c>
-      <c r="J20" s="4">
-        <f>H20/12 *300</f>
+      <c r="K21" s="4">
+        <f>I21/12 *300</f>
         <v>450</v>
       </c>
-      <c r="K20" s="1">
-        <f>(J20+$B$6)*$B$3</f>
+      <c r="L21" s="1">
+        <f>(K21+$C$7)*$C$4</f>
         <v>118.386</v>
       </c>
-      <c r="L20" s="1">
-        <f>60*H20/2*PI()*$B$3</f>
+      <c r="M21" s="1">
+        <f>60*I21/2*PI()*$C$4</f>
         <v>424.11500823462205</v>
       </c>
-      <c r="M20" s="1">
-        <f>K20*L20*PI()/30</f>
+      <c r="N21" s="1">
+        <f>L21*M21*PI()/30</f>
         <v>5257.9034398231406</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H21" s="4">
-        <f>H20+1</f>
+    <row r="22" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I22" s="4">
+        <f>I21+1</f>
         <v>19</v>
       </c>
-      <c r="I21" s="1">
-        <f>H21 * 3.6</f>
+      <c r="J22" s="1">
+        <f>I22 * 3.6</f>
         <v>68.400000000000006</v>
       </c>
-      <c r="J21" s="4">
-        <f>H21/12 *300</f>
+      <c r="K22" s="4">
+        <f>I22/12 *300</f>
         <v>475</v>
       </c>
-      <c r="K21" s="1">
-        <f>(J21+$B$6)*$B$3</f>
+      <c r="L22" s="1">
+        <f>(K22+$C$7)*$C$4</f>
         <v>124.636</v>
       </c>
-      <c r="L21" s="1">
-        <f>60*H21/2*PI()*$B$3</f>
+      <c r="M22" s="1">
+        <f>60*I22/2*PI()*$C$4</f>
         <v>447.67695313654554</v>
       </c>
-      <c r="M21" s="1">
-        <f>K21*L21*PI()/30</f>
+      <c r="N22" s="1">
+        <f>L22*M22*PI()/30</f>
         <v>5843.0130671373227</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="5">
-        <f>B16*B17*PI()/30</f>
-        <v>1379.8299128986987</v>
-      </c>
-      <c r="D22" s="15"/>
-      <c r="H22" s="4">
-        <f>H21+1</f>
+    <row r="23" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C23" s="5">
+        <f>C17*C18*PI()/30</f>
+        <v>1687.3569164322421</v>
+      </c>
+      <c r="E23" s="15"/>
+      <c r="I23" s="4">
+        <f>I22+1</f>
         <v>20</v>
       </c>
-      <c r="I22" s="1">
-        <f>H22 * 3.6</f>
+      <c r="J23" s="1">
+        <f>I23 * 3.6</f>
         <v>72</v>
       </c>
-      <c r="J22" s="4">
-        <f>H22/12 *300</f>
+      <c r="K23" s="4">
+        <f>I23/12 *300</f>
         <v>500</v>
       </c>
-      <c r="K22" s="1">
-        <f>(J22+$B$6)*$B$3</f>
+      <c r="L23" s="1">
+        <f>(K23+$C$7)*$C$4</f>
         <v>130.886</v>
       </c>
-      <c r="L22" s="1">
-        <f>60*H22/2*PI()*$B$3</f>
+      <c r="M23" s="1">
+        <f>60*I23/2*PI()*$C$4</f>
         <v>471.23889803846896</v>
       </c>
-      <c r="M22" s="1">
-        <f>K22*L22*PI()/30</f>
+      <c r="N23" s="1">
+        <f>L23*M23*PI()/30</f>
         <v>6458.9652082049079</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="5" t="s">
+    <row r="24" spans="2:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="2:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="2:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C26" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="D26" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="E26" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="F26" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="G26" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I30" s="11"/>
-    </row>
-    <row r="31" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" spans="18:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" spans="18:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" spans="18:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" spans="18:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" spans="18:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" spans="18:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="R38" t="s">
+    <row r="27" spans="2:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="2:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="2:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="2:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J31" s="11"/>
+    </row>
+    <row r="32" spans="2:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" spans="19:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" spans="19:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" spans="19:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="19:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="19:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="19:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="19:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S39" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="D12:F12"/>
   </mergeCells>
-  <conditionalFormatting sqref="A21">
+  <conditionalFormatting sqref="B22">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Continued to try to fix the caclulations, concluded they were very buggy and badly made. Next commit will begin work on a new version
</commit_message>
<xml_diff>
--- a/Motor_calculations/Car calculations.xlsx
+++ b/Motor_calculations/Car calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ronitbhandari/Desktop/VELOX/Motor_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85A632B0-AB48-D349-95F2-DF04980CA407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E10C3D-E4D0-B543-8F49-5B7A76A53242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="740" windowWidth="24960" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,40 +30,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Ronit Bhandari</author>
-  </authors>
-  <commentList>
-    <comment ref="K23" authorId="0" shapeId="0" xr:uid="{7BEA248F-B2AE-5241-843D-678136970A79}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ronit Bhandari:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
@@ -89,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>Quantity</t>
   </si>
@@ -204,10 +170,13 @@
     <t>/30</t>
   </si>
   <si>
-    <t>Closes Power Rating</t>
-  </si>
-  <si>
     <t>tire radius (m)</t>
+  </si>
+  <si>
+    <t>*3.6 (conversion)</t>
+  </si>
+  <si>
+    <t>Closest Power Rating</t>
   </si>
 </sst>
 </file>
@@ -215,9 +184,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="#,##0.000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -253,19 +222,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -407,7 +363,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -445,28 +401,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -474,23 +415,32 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -498,6 +448,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -527,7 +480,9 @@
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="velocity (m/s) (TARGET VALUE)"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="(REQUIRED) velocity (km/h)"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="(REQUIRED) Thrust force (N)"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="(REQUIRED) Thrust force (N)">
+      <calculatedColumnFormula>I3/$C$5 *$C$3</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="(REQUIRED) Torque (Nm)"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="(REQUIRED) RPM"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="(REQUIRED) Power (W)" dataDxfId="0">
@@ -833,14 +788,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="B2:S39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="91" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -895,7 +850,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="4">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -909,35 +864,35 @@
         <v>0</v>
       </c>
       <c r="K3" s="4">
-        <f t="shared" ref="K3:K12" si="1">I3/12 *300</f>
+        <f>I3/$C$5 *$C$3</f>
         <v>0</v>
       </c>
       <c r="L3" s="1">
-        <f t="shared" ref="L3:L12" si="2">(K3+$C$7)*$C$4</f>
-        <v>5.8860000000000001</v>
+        <f t="shared" ref="L3:L12" si="1">(K3+$C$7)*$C$4</f>
+        <v>36.787500000000001</v>
       </c>
       <c r="M3" s="4">
-        <f t="shared" ref="M3:M12" si="3">60*I3/2*PI()*$C$4</f>
+        <f t="shared" ref="M3:M12" si="2">60*I3/2*PI()*$C$4</f>
         <v>0</v>
       </c>
       <c r="N3" s="1">
-        <f t="shared" ref="N3:N12" si="4">L3*M3*PI()/30</f>
+        <f t="shared" ref="N3:N12" si="3">L3*M3*PI()/30</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" s="1">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="I4" s="4">
-        <f t="shared" ref="I4:I24" si="5">I3+1</f>
+        <f t="shared" ref="I4:I12" si="4">I3+1</f>
         <v>1</v>
       </c>
       <c r="J4" s="1">
@@ -945,20 +900,20 @@
         <v>3.6</v>
       </c>
       <c r="K4" s="4">
+        <f t="shared" ref="K4:K23" si="5">I4/$C$5 *$C$3</f>
+        <v>25</v>
+      </c>
+      <c r="L4" s="1">
         <f t="shared" si="1"/>
-        <v>25</v>
-      </c>
-      <c r="L4" s="1">
+        <v>39.912500000000001</v>
+      </c>
+      <c r="M4" s="1">
         <f t="shared" si="2"/>
-        <v>12.135999999999999</v>
-      </c>
-      <c r="M4" s="1">
+        <v>11.780972450961723</v>
+      </c>
+      <c r="N4" s="1">
         <f t="shared" si="3"/>
-        <v>23.561944901923447</v>
-      </c>
-      <c r="N4" s="1">
-        <f t="shared" si="4"/>
-        <v>29.944379752905107</v>
+        <v>49.240073207309869</v>
       </c>
     </row>
     <row r="5" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -973,7 +928,7 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="I5" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="J5" s="1">
@@ -981,20 +936,20 @@
         <v>7.2</v>
       </c>
       <c r="K5" s="4">
+        <f t="shared" si="5"/>
+        <v>50</v>
+      </c>
+      <c r="L5" s="1">
         <f t="shared" si="1"/>
-        <v>50</v>
-      </c>
-      <c r="L5" s="1">
+        <v>43.037500000000001</v>
+      </c>
+      <c r="M5" s="1">
         <f t="shared" si="2"/>
-        <v>18.385999999999999</v>
-      </c>
-      <c r="M5" s="1">
+        <v>23.561944901923447</v>
+      </c>
+      <c r="N5" s="1">
         <f t="shared" si="3"/>
-        <v>47.123889803846893</v>
-      </c>
-      <c r="N5" s="1">
-        <f t="shared" si="4"/>
-        <v>90.731273259214461</v>
+        <v>106.1907748529708</v>
       </c>
     </row>
     <row r="6" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1002,14 +957,14 @@
         <v>10</v>
       </c>
       <c r="C6" s="1">
-        <v>1.2E-2</v>
+        <v>0.1</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="I6" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="J6" s="1">
@@ -1017,20 +972,20 @@
         <v>10.8</v>
       </c>
       <c r="K6" s="4">
+        <f t="shared" si="5"/>
+        <v>75</v>
+      </c>
+      <c r="L6" s="1">
         <f t="shared" si="1"/>
-        <v>75</v>
-      </c>
-      <c r="L6" s="1">
+        <v>46.162500000000001</v>
+      </c>
+      <c r="M6" s="1">
         <f t="shared" si="2"/>
-        <v>24.635999999999999</v>
-      </c>
-      <c r="M6" s="1">
+        <v>35.342917352885173</v>
+      </c>
+      <c r="N6" s="1">
         <f t="shared" si="3"/>
-        <v>70.685834705770347</v>
-      </c>
-      <c r="N6" s="1">
-        <f t="shared" si="4"/>
-        <v>182.36068051892804</v>
+        <v>170.85210493698284</v>
       </c>
     </row>
     <row r="7" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1039,14 +994,14 @@
       </c>
       <c r="C7" s="1">
         <f>C3*9.81*C6</f>
-        <v>23.544</v>
+        <v>294.3</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="I7" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="J7" s="1">
@@ -1054,25 +1009,25 @@
         <v>14.4</v>
       </c>
       <c r="K7" s="4">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+      <c r="L7" s="1">
         <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="L7" s="1">
+        <v>49.287500000000001</v>
+      </c>
+      <c r="M7" s="1">
         <f t="shared" si="2"/>
-        <v>30.885999999999999</v>
-      </c>
-      <c r="M7" s="1">
+        <v>47.123889803846893</v>
+      </c>
+      <c r="N7" s="1">
         <f t="shared" si="3"/>
-        <v>94.247779607693786</v>
-      </c>
-      <c r="N7" s="1">
-        <f t="shared" si="4"/>
-        <v>304.83260153204589</v>
+        <v>243.22406345934584</v>
       </c>
     </row>
     <row r="8" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I8" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="J8" s="1">
@@ -1080,25 +1035,25 @@
         <v>18</v>
       </c>
       <c r="K8" s="4">
+        <f t="shared" si="5"/>
+        <v>125</v>
+      </c>
+      <c r="L8" s="1">
         <f t="shared" si="1"/>
-        <v>125</v>
-      </c>
-      <c r="L8" s="1">
+        <v>52.412500000000001</v>
+      </c>
+      <c r="M8" s="1">
         <f t="shared" si="2"/>
-        <v>37.136000000000003</v>
-      </c>
-      <c r="M8" s="1">
+        <v>58.90486225480862</v>
+      </c>
+      <c r="N8" s="1">
         <f t="shared" si="3"/>
-        <v>117.80972450961724</v>
-      </c>
-      <c r="N8" s="1">
-        <f t="shared" si="4"/>
-        <v>458.14703629856803</v>
+        <v>323.30665042005995</v>
       </c>
     </row>
     <row r="9" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I9" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="J9" s="1">
@@ -1106,25 +1061,25 @@
         <v>21.6</v>
       </c>
       <c r="K9" s="4">
+        <f t="shared" si="5"/>
+        <v>150</v>
+      </c>
+      <c r="L9" s="1">
         <f t="shared" si="1"/>
-        <v>150</v>
-      </c>
-      <c r="L9" s="1">
+        <v>55.537500000000001</v>
+      </c>
+      <c r="M9" s="1">
         <f t="shared" si="2"/>
-        <v>43.386000000000003</v>
-      </c>
-      <c r="M9" s="1">
+        <v>70.685834705770347</v>
+      </c>
+      <c r="N9" s="1">
         <f t="shared" si="3"/>
-        <v>141.37166941154069</v>
-      </c>
-      <c r="N9" s="1">
-        <f t="shared" si="4"/>
-        <v>642.30398481849443</v>
+        <v>411.09986581912523</v>
       </c>
     </row>
     <row r="10" spans="2:14" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="I10" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="J10" s="1">
@@ -1132,33 +1087,33 @@
         <v>25.2</v>
       </c>
       <c r="K10" s="4">
+        <f t="shared" si="5"/>
+        <v>175</v>
+      </c>
+      <c r="L10" s="1">
         <f t="shared" si="1"/>
-        <v>175</v>
-      </c>
-      <c r="L10" s="1">
+        <v>58.662500000000001</v>
+      </c>
+      <c r="M10" s="1">
         <f t="shared" si="2"/>
-        <v>49.636000000000003</v>
-      </c>
-      <c r="M10" s="1">
+        <v>82.466807156732074</v>
+      </c>
+      <c r="N10" s="1">
         <f t="shared" si="3"/>
-        <v>164.93361431346415</v>
-      </c>
-      <c r="N10" s="1">
+        <v>506.60370965654141</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="16"/>
+      <c r="I11" s="4">
         <f t="shared" si="4"/>
-        <v>857.30344709182498</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="17"/>
-      <c r="I11" s="4">
-        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="J11" s="1">
@@ -1166,35 +1121,35 @@
         <v>28.8</v>
       </c>
       <c r="K11" s="4">
+        <f t="shared" si="5"/>
+        <v>200</v>
+      </c>
+      <c r="L11" s="1">
         <f t="shared" si="1"/>
-        <v>200</v>
-      </c>
-      <c r="L11" s="1">
+        <v>61.787500000000001</v>
+      </c>
+      <c r="M11" s="1">
         <f t="shared" si="2"/>
-        <v>55.886000000000003</v>
-      </c>
-      <c r="M11" s="1">
+        <v>94.247779607693786</v>
+      </c>
+      <c r="N11" s="1">
         <f t="shared" si="3"/>
-        <v>188.49555921538757</v>
-      </c>
-      <c r="N11" s="1">
+        <v>609.81818193230868</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="36"/>
+      <c r="D12" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="40"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="13"/>
+      <c r="I12" s="4">
         <f t="shared" si="4"/>
-        <v>1103.1454231185596</v>
-      </c>
-    </row>
-    <row r="12" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="20"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="18"/>
-      <c r="I12" s="4">
-        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="J12" s="1">
@@ -1202,403 +1157,406 @@
         <v>32.4</v>
       </c>
       <c r="K12" s="4">
+        <f t="shared" si="5"/>
+        <v>225</v>
+      </c>
+      <c r="L12" s="1">
         <f t="shared" si="1"/>
-        <v>225</v>
-      </c>
-      <c r="L12" s="1">
+        <v>64.912499999999994</v>
+      </c>
+      <c r="M12" s="1">
         <f t="shared" si="2"/>
-        <v>62.136000000000003</v>
-      </c>
-      <c r="M12" s="1">
+        <v>106.02875205865551</v>
+      </c>
+      <c r="N12" s="1">
         <f t="shared" si="3"/>
-        <v>212.05750411731103</v>
-      </c>
-      <c r="N12" s="1">
-        <f t="shared" si="4"/>
-        <v>1379.8299128986987</v>
+        <v>720.74328264642691</v>
       </c>
     </row>
     <row r="13" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="38" t="s">
+      <c r="B13" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="30">
-        <v>1687.36</v>
-      </c>
-      <c r="D13" s="22"/>
+      <c r="C13" s="23">
+        <v>1800</v>
+      </c>
+      <c r="D13" s="17"/>
       <c r="E13" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="35" t="s">
+      <c r="F13" s="27" t="s">
         <v>27</v>
       </c>
       <c r="I13" s="7">
-        <f>I12+1</f>
+        <f t="shared" ref="I13:I23" si="6">I12+1</f>
         <v>10</v>
       </c>
       <c r="J13" s="8">
-        <f>I13 * 3.6</f>
+        <f t="shared" ref="J13:J23" si="7">I13 * 3.6</f>
         <v>36</v>
       </c>
-      <c r="K13" s="7">
-        <f>I13/12 *300</f>
+      <c r="K13" s="4">
+        <f t="shared" si="5"/>
         <v>250</v>
       </c>
       <c r="L13" s="8">
-        <f>(K13+$C$7)*$C$4</f>
-        <v>68.385999999999996</v>
+        <f t="shared" ref="L13:L23" si="8">(K13+$C$7)*$C$4</f>
+        <v>68.037499999999994</v>
       </c>
       <c r="M13" s="8">
-        <f>60*I13/2*PI()*$C$4</f>
-        <v>235.61944901923448</v>
+        <f t="shared" ref="M13:M23" si="9">60*I13/2*PI()*$C$4</f>
+        <v>117.80972450961724</v>
       </c>
       <c r="N13" s="1">
-        <f>L13*M13*PI()/30</f>
-        <v>1687.3569164322421</v>
+        <f t="shared" ref="N13:N23" si="10">L13*M13*PI()/30</f>
+        <v>839.37901179889639</v>
       </c>
     </row>
     <row r="14" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="39" t="s">
+      <c r="B14" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="30">
-        <v>2000</v>
-      </c>
-      <c r="D14" s="23" t="s">
+      <c r="C14" s="23">
+        <v>4500</v>
+      </c>
+      <c r="D14" s="18" t="s">
         <v>23</v>
       </c>
       <c r="E14" s="9"/>
-      <c r="F14" s="34"/>
+      <c r="F14" s="26"/>
       <c r="H14" s="6"/>
       <c r="I14" s="4">
-        <f>I13+1</f>
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
       <c r="J14" s="1">
-        <f>I14 * 3.6</f>
+        <f t="shared" si="7"/>
         <v>39.6</v>
       </c>
       <c r="K14" s="4">
-        <f>I14/12 *300</f>
+        <f t="shared" si="5"/>
         <v>275</v>
       </c>
       <c r="L14" s="1">
-        <f>(K14+$C$7)*$C$4</f>
-        <v>74.635999999999996</v>
+        <f t="shared" si="8"/>
+        <v>71.162499999999994</v>
       </c>
       <c r="M14" s="1">
-        <f>60*I14/2*PI()*$C$4</f>
-        <v>259.18139392115791</v>
+        <f t="shared" si="9"/>
+        <v>129.59069696057895</v>
       </c>
       <c r="N14" s="1">
-        <f>L14*M14*PI()/30</f>
-        <v>2025.7264337191891</v>
+        <f t="shared" si="10"/>
+        <v>965.72536938971678</v>
       </c>
     </row>
     <row r="15" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="39" t="s">
+      <c r="B15" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="30">
-        <f>9550*C13/C14</f>
-        <v>8057.1439999999993</v>
-      </c>
-      <c r="D15" s="24" t="s">
+      <c r="C15" s="23">
+        <f>(30/PI())*C13/C14</f>
+        <v>3.819718634205489</v>
+      </c>
+      <c r="D15" s="19" t="s">
         <v>24</v>
       </c>
       <c r="E15" s="9"/>
-      <c r="F15" s="33"/>
+      <c r="F15" s="25"/>
       <c r="I15" s="4">
-        <f>I14+1</f>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="J15" s="1">
-        <f>I15 * 3.6</f>
+        <f t="shared" si="7"/>
         <v>43.2</v>
       </c>
       <c r="K15" s="4">
-        <f>I15/12 *300</f>
+        <f t="shared" si="5"/>
         <v>300</v>
       </c>
       <c r="L15" s="1">
-        <f>(K15+$C$7)*$C$4</f>
-        <v>80.885999999999996</v>
+        <f t="shared" si="8"/>
+        <v>74.287499999999994</v>
       </c>
       <c r="M15" s="1">
-        <f>60*I15/2*PI()*$C$4</f>
-        <v>282.74333882308139</v>
+        <f t="shared" si="9"/>
+        <v>141.37166941154069</v>
       </c>
       <c r="N15" s="1">
-        <f>L15*M15*PI()/30</f>
-        <v>2394.9384647595411</v>
+        <f t="shared" si="10"/>
+        <v>1099.7823554188883</v>
       </c>
     </row>
     <row r="16" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="35" t="s">
         <v>25</v>
       </c>
       <c r="C16" s="36"/>
-      <c r="D16" s="24" t="s">
+      <c r="D16" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="F16" s="30"/>
+      <c r="F16" s="23"/>
       <c r="I16" s="4">
-        <f>I15+1</f>
+        <f t="shared" si="6"/>
         <v>13</v>
       </c>
       <c r="J16" s="1">
-        <f>I16 * 3.6</f>
+        <f t="shared" si="7"/>
         <v>46.800000000000004</v>
       </c>
       <c r="K16" s="4">
-        <f>I16/12 *300</f>
+        <f t="shared" si="5"/>
         <v>325</v>
       </c>
       <c r="L16" s="1">
-        <f>(K16+$C$7)*$C$4</f>
-        <v>87.135999999999996</v>
+        <f t="shared" si="8"/>
+        <v>77.412499999999994</v>
       </c>
       <c r="M16" s="1">
-        <f>60*I16/2*PI()*$C$4</f>
-        <v>306.30528372500481</v>
+        <f t="shared" si="9"/>
+        <v>153.15264186250241</v>
       </c>
       <c r="N16" s="1">
-        <f>L16*M16*PI()/30</f>
-        <v>2794.9930095532973</v>
+        <f t="shared" si="10"/>
+        <v>1241.549969886411</v>
       </c>
     </row>
     <row r="17" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="39" t="s">
+      <c r="B17" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="30" cm="1">
+      <c r="C17" s="23" cm="1">
         <f t="array" ref="C17">INDEX(Table1[(REQUIRED) RPM],MATCH(MIN(ABS(Table1[(REQUIRED) Power (W)]- C13)), ABS(Table1[(REQUIRED) Power (W)]- C13), 0))</f>
-        <v>235.61944901923448</v>
-      </c>
-      <c r="D17" s="26" t="s">
+        <v>200.27653166634931</v>
+      </c>
+      <c r="D17" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="21"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="19"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="15"/>
       <c r="I17" s="4">
-        <f>I16+1</f>
+        <f t="shared" si="6"/>
         <v>14</v>
       </c>
       <c r="J17" s="1">
-        <f>I17 * 3.6</f>
+        <f t="shared" si="7"/>
         <v>50.4</v>
       </c>
       <c r="K17" s="4">
-        <f>I17/12 *300</f>
+        <f t="shared" si="5"/>
         <v>350</v>
       </c>
       <c r="L17" s="1">
-        <f>(K17+$C$7)*$C$4</f>
-        <v>93.385999999999996</v>
+        <f t="shared" si="8"/>
+        <v>80.537499999999994</v>
       </c>
       <c r="M17" s="1">
-        <f>60*I17/2*PI()*$C$4</f>
-        <v>329.86722862692829</v>
+        <f t="shared" si="9"/>
+        <v>164.93361431346415</v>
       </c>
       <c r="N17" s="1">
-        <f>L17*M17*PI()/30</f>
-        <v>3225.8900681004575</v>
+        <f t="shared" si="10"/>
+        <v>1391.0282127922849</v>
       </c>
     </row>
     <row r="18" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="39" t="s">
+      <c r="B18" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="30" cm="1">
+      <c r="C18" s="23" cm="1">
         <f t="array" ref="C18">INDEX(Table1[(REQUIRED) Torque (Nm)],MATCH(MIN(ABS(Table1[(REQUIRED) Power (W)]- C13)), ABS(Table1[(REQUIRED) Power (W)]- C13), 0))</f>
-        <v>68.385999999999996</v>
-      </c>
-      <c r="D18" s="37"/>
-      <c r="E18" s="16" t="s">
+        <v>89.912499999999994</v>
+      </c>
+      <c r="D18" s="28"/>
+      <c r="E18" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="F18" s="31" t="s">
+      <c r="F18" s="24" t="s">
         <v>24</v>
       </c>
       <c r="I18" s="4">
-        <f>I17+1</f>
+        <f t="shared" si="6"/>
         <v>15</v>
       </c>
       <c r="J18" s="1">
-        <f>I18 * 3.6</f>
+        <f t="shared" si="7"/>
         <v>54</v>
       </c>
       <c r="K18" s="4">
-        <f>I18/12 *300</f>
+        <f t="shared" si="5"/>
         <v>375</v>
       </c>
       <c r="L18" s="1">
-        <f>(K18+$C$7)*$C$4</f>
-        <v>99.635999999999996</v>
+        <f t="shared" si="8"/>
+        <v>83.662499999999994</v>
       </c>
       <c r="M18" s="1">
-        <f>60*I18/2*PI()*$C$4</f>
-        <v>353.42917352885172</v>
+        <f t="shared" si="9"/>
+        <v>176.71458676442586</v>
       </c>
       <c r="N18" s="1">
-        <f>L18*M18*PI()/30</f>
-        <v>3687.6296404010222</v>
+        <f t="shared" si="10"/>
+        <v>1548.2170841365094</v>
       </c>
     </row>
     <row r="19" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="29" cm="1">
+      <c r="B19" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="22" cm="1">
         <f t="array" ref="C19">INDEX(Table1[(REQUIRED) Power (W)],MATCH(MIN(ABS(Table1[(REQUIRED) Power (W)]- C13)), ABS(Table1[(REQUIRED) Power (W)]- C13), 0))</f>
-        <v>1687.3569164322421</v>
-      </c>
-      <c r="D19" s="24" t="s">
+        <v>1885.7267121400121</v>
+      </c>
+      <c r="D19" s="19" t="s">
         <v>17</v>
       </c>
       <c r="E19" s="12"/>
-      <c r="F19" s="30"/>
+      <c r="F19" s="23"/>
       <c r="I19" s="4">
-        <f>I18+1</f>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="J19" s="1">
-        <f>I19 * 3.6</f>
+        <f t="shared" si="7"/>
         <v>57.6</v>
       </c>
       <c r="K19" s="4">
-        <f>I19/12 *300</f>
+        <f t="shared" si="5"/>
         <v>400</v>
       </c>
       <c r="L19" s="1">
-        <f>(K19+$C$7)*$C$4</f>
-        <v>105.886</v>
+        <f t="shared" si="8"/>
+        <v>86.787499999999994</v>
       </c>
       <c r="M19" s="1">
-        <f>60*I19/2*PI()*$C$4</f>
-        <v>376.99111843077515</v>
+        <f t="shared" si="9"/>
+        <v>188.49555921538757</v>
       </c>
       <c r="N19" s="1">
-        <f>L19*M19*PI()/30</f>
-        <v>4180.2117264549906</v>
+        <f t="shared" si="10"/>
+        <v>1713.1165839190851</v>
       </c>
     </row>
     <row r="20" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="13"/>
-      <c r="D20" s="27" t="s">
+      <c r="D20" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="E20" s="28"/>
-      <c r="F20" s="29"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="22"/>
       <c r="I20" s="4">
-        <f>I19+1</f>
+        <f t="shared" si="6"/>
         <v>17</v>
       </c>
       <c r="J20" s="1">
-        <f>I20 * 3.6</f>
+        <f t="shared" si="7"/>
         <v>61.2</v>
       </c>
       <c r="K20" s="4">
-        <f>I20/12 *300</f>
+        <f t="shared" si="5"/>
         <v>425</v>
       </c>
       <c r="L20" s="1">
-        <f>(K20+$C$7)*$C$4</f>
-        <v>112.136</v>
+        <f t="shared" si="8"/>
+        <v>89.912499999999994</v>
       </c>
       <c r="M20" s="1">
-        <f>60*I20/2*PI()*$C$4</f>
-        <v>400.55306333269863</v>
+        <f t="shared" si="9"/>
+        <v>200.27653166634931</v>
       </c>
       <c r="N20" s="1">
-        <f>L20*M20*PI()/30</f>
-        <v>4703.6363262623645</v>
+        <f t="shared" si="10"/>
+        <v>1885.7267121400121</v>
       </c>
     </row>
     <row r="21" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="13"/>
-      <c r="D21" s="37"/>
+      <c r="D21" s="28"/>
       <c r="I21" s="4">
-        <f>I20+1</f>
+        <f t="shared" si="6"/>
         <v>18</v>
       </c>
       <c r="J21" s="1">
-        <f>I21 * 3.6</f>
+        <f t="shared" si="7"/>
         <v>64.8</v>
       </c>
       <c r="K21" s="4">
-        <f>I21/12 *300</f>
+        <f t="shared" si="5"/>
         <v>450</v>
       </c>
       <c r="L21" s="1">
-        <f>(K21+$C$7)*$C$4</f>
-        <v>118.386</v>
+        <f t="shared" si="8"/>
+        <v>93.037499999999994</v>
       </c>
       <c r="M21" s="1">
-        <f>60*I21/2*PI()*$C$4</f>
-        <v>424.11500823462205</v>
+        <f t="shared" si="9"/>
+        <v>212.05750411731103</v>
       </c>
       <c r="N21" s="1">
-        <f>L21*M21*PI()/30</f>
-        <v>5257.9034398231406</v>
+        <f t="shared" si="10"/>
+        <v>2066.0474687992896</v>
       </c>
     </row>
     <row r="22" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I22" s="4">
-        <f>I21+1</f>
+        <f t="shared" si="6"/>
         <v>19</v>
       </c>
       <c r="J22" s="1">
-        <f>I22 * 3.6</f>
+        <f t="shared" si="7"/>
         <v>68.400000000000006</v>
       </c>
       <c r="K22" s="4">
-        <f>I22/12 *300</f>
+        <f t="shared" si="5"/>
         <v>475</v>
       </c>
       <c r="L22" s="1">
-        <f>(K22+$C$7)*$C$4</f>
-        <v>124.636</v>
+        <f t="shared" si="8"/>
+        <v>96.162499999999994</v>
       </c>
       <c r="M22" s="1">
-        <f>60*I22/2*PI()*$C$4</f>
-        <v>447.67695313654554</v>
+        <f t="shared" si="9"/>
+        <v>223.83847656827277</v>
       </c>
       <c r="N22" s="1">
-        <f>L22*M22*PI()/30</f>
-        <v>5843.0130671373227</v>
+        <f t="shared" si="10"/>
+        <v>2254.0788538969191</v>
       </c>
     </row>
     <row r="23" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C23" s="5">
         <f>C17*C18*PI()/30</f>
-        <v>1687.3569164322421</v>
-      </c>
-      <c r="E23" s="15"/>
+        <v>1885.7267121400121</v>
+      </c>
+      <c r="E23" s="5">
+        <f>3.82*15</f>
+        <v>57.3</v>
+      </c>
       <c r="I23" s="4">
-        <f>I22+1</f>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="J23" s="1">
-        <f>I23 * 3.6</f>
+        <f t="shared" si="7"/>
         <v>72</v>
       </c>
       <c r="K23" s="4">
-        <f>I23/12 *300</f>
+        <f>I23/$C$5 *$C$3</f>
         <v>500</v>
       </c>
       <c r="L23" s="1">
-        <f>(K23+$C$7)*$C$4</f>
-        <v>130.886</v>
+        <f t="shared" si="8"/>
+        <v>99.287499999999994</v>
       </c>
       <c r="M23" s="1">
-        <f>60*I23/2*PI()*$C$4</f>
-        <v>471.23889803846896</v>
+        <f t="shared" si="9"/>
+        <v>235.61944901923448</v>
       </c>
       <c r="N23" s="1">
-        <f>L23*M23*PI()/30</f>
-        <v>6458.9652082049079</v>
+        <f t="shared" si="10"/>
+        <v>2449.8208674328989</v>
       </c>
     </row>
     <row r="24" spans="2:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1618,6 +1576,9 @@
       </c>
       <c r="G26" s="5" t="s">
         <v>32</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="2:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1657,10 +1618,9 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
   <tableParts count="2">
+    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>